<commit_message>
last updated test data
</commit_message>
<xml_diff>
--- a/data/fake_emdat_test.xlsx
+++ b/data/fake_emdat_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43E46F-A7FF-488B-84B0-1746CC7E195F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C23468C-2F4E-447B-828B-ED19DC572095}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2215,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K49" workbookViewId="0">
-      <selection activeCell="U63" sqref="U63"/>
+    <sheetView tabSelected="1" topLeftCell="K40" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Last updated test data with invalid GAUL codes
</commit_message>
<xml_diff>
--- a/data/fake_emdat_test.xlsx
+++ b/data/fake_emdat_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E5CE77-2843-4ACE-A109-138522F80D8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE1AA43-1503-4ED6-95A9-6BB43AC08AD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3660" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="626">
   <si>
     <t>Source:</t>
   </si>
@@ -1251,9 +1251,6 @@
     <t>Taiwan Sheng province</t>
   </si>
   <si>
-    <t>[{"adm1_code":925,"adm1_name":"Taiwan Sheng"}]</t>
-  </si>
-  <si>
     <t>Hainan Sheng province</t>
   </si>
   <si>
@@ -1386,9 +1383,6 @@
     <t>Manoa Valley area (Honolulu district, Hawaii province)</t>
   </si>
   <si>
-    <t>[{"adm2_code":29225,"adm2_name":"Honolulu"}]</t>
-  </si>
-  <si>
     <t>[{"adm1_code":1512,"adm1_name":"Nangroe Aceh Darussalam"},{"adm1_code":1537,"adm1_name":"Sumatera Utara"}]</t>
   </si>
   <si>
@@ -1897,6 +1891,12 @@
   </si>
   <si>
     <t>1927-0013-DZA</t>
+  </si>
+  <si>
+    <t>[{"adm1_code":19888,"adm1_name":"Taiwan Sheng"}]</t>
+  </si>
+  <si>
+    <t>[{"adm2_code":198888,"adm2_name":"Honolulu"}]</t>
   </si>
 </sst>
 </file>
@@ -2225,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="U83" sqref="U83"/>
+    <sheetView tabSelected="1" topLeftCell="M31" workbookViewId="0">
+      <selection activeCell="AR61" sqref="AR61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,6 +2248,7 @@
     <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -2392,7 +2393,7 @@
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -2535,7 +2536,7 @@
         <v>372</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C3" t="s">
         <v>209</v>
@@ -2678,7 +2679,7 @@
         <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -2812,7 +2813,7 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
@@ -2821,7 +2822,7 @@
         <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E5" t="s">
         <v>78</v>
@@ -2833,16 +2834,16 @@
         <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I5" t="s">
         <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L5" t="s">
         <v>140</v>
@@ -2851,7 +2852,7 @@
         <v>114</v>
       </c>
       <c r="N5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="O5" t="s">
         <v>65</v>
@@ -2941,10 +2942,10 @@
         <v>83.90417006010567</v>
       </c>
       <c r="AR5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AS5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="AT5" t="s">
         <v>76</v>
@@ -2952,7 +2953,7 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B6" t="s">
         <v>70</v>
@@ -2964,7 +2965,7 @@
         <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F6" t="s">
         <v>84</v>
@@ -2991,7 +2992,7 @@
         <v>107</v>
       </c>
       <c r="N6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="O6" t="s">
         <v>65</v>
@@ -3084,7 +3085,7 @@
         <v>65</v>
       </c>
       <c r="AS6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AT6" t="s">
         <v>76</v>
@@ -3107,7 +3108,7 @@
         <v>132</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="G7" t="s">
         <v>254</v>
@@ -3250,7 +3251,7 @@
         <v>157</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H8" t="s">
         <v>65</v>
@@ -3372,7 +3373,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -3393,7 +3394,7 @@
         <v>278</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="I9" t="s">
         <v>65</v>
@@ -3411,7 +3412,7 @@
         <v>92</v>
       </c>
       <c r="N9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O9" t="s">
         <v>65</v>
@@ -3509,7 +3510,7 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -3536,7 +3537,7 @@
         <v>65</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K10" t="s">
         <v>147</v>
@@ -3548,7 +3549,7 @@
         <v>69</v>
       </c>
       <c r="N10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="O10" t="s">
         <v>65</v>
@@ -3641,7 +3642,7 @@
         <v>65</v>
       </c>
       <c r="AS10" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="AT10" t="s">
         <v>76</v>
@@ -3679,7 +3680,7 @@
         <v>103</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L11" t="s">
         <v>105</v>
@@ -3789,7 +3790,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -3822,13 +3823,13 @@
         <v>329</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="M12" t="s">
         <v>114</v>
       </c>
       <c r="N12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="O12" t="s">
         <v>65</v>
@@ -3929,7 +3930,7 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
@@ -3965,7 +3966,7 @@
         <v>166</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="N13" t="s">
         <v>214</v>
@@ -4069,7 +4070,7 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B14" t="s">
         <v>70</v>
@@ -4090,7 +4091,7 @@
         <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I14" t="s">
         <v>65</v>
@@ -4108,7 +4109,7 @@
         <v>69</v>
       </c>
       <c r="N14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="O14" t="s">
         <v>65</v>
@@ -4117,7 +4118,7 @@
         <v>63</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="R14" t="s">
         <v>70</v>
@@ -4198,10 +4199,10 @@
         <v>83.90417006010567</v>
       </c>
       <c r="AR14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AS14" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="AT14" t="s">
         <v>76</v>
@@ -4209,7 +4210,7 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -4233,7 +4234,7 @@
         <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J15" t="s">
         <v>240</v>
@@ -4248,7 +4249,7 @@
         <v>114</v>
       </c>
       <c r="N15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="O15" t="s">
         <v>65</v>
@@ -4260,7 +4261,7 @@
         <v>70</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="S15" t="s">
         <v>70</v>
@@ -4338,10 +4339,10 @@
         <v>77.78656765992335</v>
       </c>
       <c r="AR15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AS15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AT15" t="s">
         <v>76</v>
@@ -4349,7 +4350,7 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
@@ -4388,7 +4389,7 @@
         <v>92</v>
       </c>
       <c r="N16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="O16" t="s">
         <v>65</v>
@@ -4403,7 +4404,7 @@
         <v>70</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="T16" t="s">
         <v>65</v>
@@ -4481,7 +4482,7 @@
         <v>65</v>
       </c>
       <c r="AS16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AT16" t="s">
         <v>76</v>
@@ -4489,7 +4490,7 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B17" t="s">
         <v>70</v>
@@ -4528,7 +4529,7 @@
         <v>114</v>
       </c>
       <c r="N17" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="O17" t="s">
         <v>298</v>
@@ -4618,10 +4619,10 @@
         <v>88.929493477207373</v>
       </c>
       <c r="AR17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="AS17" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AT17" t="s">
         <v>76</v>
@@ -4629,7 +4630,7 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B18" t="s">
         <v>70</v>
@@ -4653,7 +4654,7 @@
         <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J18" t="s">
         <v>367</v>
@@ -4668,7 +4669,7 @@
         <v>114</v>
       </c>
       <c r="N18" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O18" t="s">
         <v>65</v>
@@ -4761,7 +4762,7 @@
         <v>65</v>
       </c>
       <c r="AS18" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AT18" t="s">
         <v>76</v>
@@ -4832,7 +4833,7 @@
         <v>65</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="W19" t="s">
         <v>65</v>
@@ -5049,7 +5050,7 @@
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B21" t="s">
         <v>70</v>
@@ -5181,7 +5182,7 @@
         <v>65</v>
       </c>
       <c r="AS21" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AT21" t="s">
         <v>76</v>
@@ -5189,7 +5190,7 @@
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B22" t="s">
         <v>70</v>
@@ -5213,7 +5214,7 @@
         <v>65</v>
       </c>
       <c r="I22" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J22" t="s">
         <v>164</v>
@@ -5228,7 +5229,7 @@
         <v>69</v>
       </c>
       <c r="N22" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="O22" t="s">
         <v>65</v>
@@ -5318,18 +5319,18 @@
         <v>96.04634212554906</v>
       </c>
       <c r="AR22" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="AS22" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="AT22" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
@@ -5368,7 +5369,7 @@
         <v>92</v>
       </c>
       <c r="N23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="O23" t="s">
         <v>65</v>
@@ -5458,10 +5459,10 @@
         <v>70.408861756934087</v>
       </c>
       <c r="AR23" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AS23" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="AT23" t="s">
         <v>76</v>
@@ -5469,7 +5470,7 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B24" t="s">
         <v>70</v>
@@ -5508,7 +5509,7 @@
         <v>92</v>
       </c>
       <c r="N24" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="O24" t="s">
         <v>65</v>
@@ -5598,10 +5599,10 @@
         <v>83.90417006010567</v>
       </c>
       <c r="AR24" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AS24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AT24" t="s">
         <v>76</v>
@@ -5749,7 +5750,7 @@
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B26" t="s">
         <v>70</v>
@@ -5773,7 +5774,7 @@
         <v>65</v>
       </c>
       <c r="I26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J26" t="s">
         <v>233</v>
@@ -5788,7 +5789,7 @@
         <v>193</v>
       </c>
       <c r="N26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O26" t="s">
         <v>65</v>
@@ -5878,7 +5879,7 @@
         <v>59.033144078614221</v>
       </c>
       <c r="AR26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AS26" t="s">
         <v>405</v>
@@ -6309,7 +6310,7 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B30" t="s">
         <v>70</v>
@@ -6348,10 +6349,10 @@
         <v>92</v>
       </c>
       <c r="N30" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="O30" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P30" t="s">
         <v>65</v>
@@ -6438,10 +6439,10 @@
         <v>76.454145985162981</v>
       </c>
       <c r="AR30" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AS30" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AT30" t="s">
         <v>76</v>
@@ -6449,7 +6450,7 @@
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B31" t="s">
         <v>70</v>
@@ -6488,7 +6489,7 @@
         <v>193</v>
       </c>
       <c r="N31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="O31" t="s">
         <v>387</v>
@@ -6578,10 +6579,10 @@
         <v>61.989585934321688</v>
       </c>
       <c r="AR31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AS31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AT31" t="s">
         <v>76</v>
@@ -6729,7 +6730,7 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B33" t="s">
         <v>70</v>
@@ -6768,7 +6769,7 @@
         <v>92</v>
       </c>
       <c r="N33" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="O33" t="s">
         <v>65</v>
@@ -6866,7 +6867,7 @@
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B34" t="s">
         <v>70</v>
@@ -6905,10 +6906,10 @@
         <v>92</v>
       </c>
       <c r="N34" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="O34" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="P34" t="s">
         <v>65</v>
@@ -6995,10 +6996,10 @@
         <v>76.454145985162981</v>
       </c>
       <c r="AR34" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AS34" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AT34" t="s">
         <v>76</v>
@@ -7146,7 +7147,7 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B36" t="s">
         <v>70</v>
@@ -7185,7 +7186,7 @@
         <v>92</v>
       </c>
       <c r="N36" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="O36" t="s">
         <v>65</v>
@@ -7278,7 +7279,7 @@
         <v>65</v>
       </c>
       <c r="AS36" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="AT36" t="s">
         <v>76</v>
@@ -7566,7 +7567,7 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B39" t="s">
         <v>70</v>
@@ -7590,7 +7591,7 @@
         <v>65</v>
       </c>
       <c r="I39" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J39" t="s">
         <v>124</v>
@@ -7706,7 +7707,7 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B40" t="s">
         <v>70</v>
@@ -7745,7 +7746,7 @@
         <v>107</v>
       </c>
       <c r="N40" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="O40" t="s">
         <v>65</v>
@@ -8115,7 +8116,7 @@
         <v>54.668220842288505</v>
       </c>
       <c r="AR42" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="AS42" t="s">
         <v>75</v>
@@ -8126,7 +8127,7 @@
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B43" t="s">
         <v>70</v>
@@ -8165,7 +8166,7 @@
         <v>114</v>
       </c>
       <c r="N43" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="O43" t="s">
         <v>65</v>
@@ -8255,10 +8256,10 @@
         <v>71.56359557518887</v>
       </c>
       <c r="AR43" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AS43" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="AT43" t="s">
         <v>76</v>
@@ -8401,12 +8402,12 @@
         <v>75</v>
       </c>
       <c r="AT44" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
@@ -8430,7 +8431,7 @@
         <v>65</v>
       </c>
       <c r="I45" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="J45" t="s">
         <v>124</v>
@@ -8445,7 +8446,7 @@
         <v>92</v>
       </c>
       <c r="N45" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="O45" t="s">
         <v>65</v>
@@ -8533,10 +8534,10 @@
         <v>76.454145985162981</v>
       </c>
       <c r="AR45" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AS45" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AT45" t="s">
         <v>76</v>
@@ -8544,7 +8545,7 @@
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
@@ -8583,7 +8584,7 @@
         <v>114</v>
       </c>
       <c r="N46" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="O46" t="s">
         <v>298</v>
@@ -8671,10 +8672,10 @@
         <v>77.78656765992335</v>
       </c>
       <c r="AR46" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AS46" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AT46" t="s">
         <v>76</v>
@@ -8682,7 +8683,7 @@
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B47" t="s">
         <v>70</v>
@@ -8721,7 +8722,7 @@
         <v>92</v>
       </c>
       <c r="N47" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="O47" t="s">
         <v>298</v>
@@ -8811,10 +8812,10 @@
         <v>88.929493477207373</v>
       </c>
       <c r="AR47" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AS47" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AT47" t="s">
         <v>76</v>
@@ -8822,7 +8823,7 @@
     </row>
     <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B48" t="s">
         <v>70</v>
@@ -8861,7 +8862,7 @@
         <v>114</v>
       </c>
       <c r="N48" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="O48" t="s">
         <v>65</v>
@@ -8954,7 +8955,7 @@
         <v>65</v>
       </c>
       <c r="AS48" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AT48" t="s">
         <v>76</v>
@@ -8962,7 +8963,7 @@
     </row>
     <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
@@ -9094,7 +9095,7 @@
         <v>65</v>
       </c>
       <c r="AS49" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AT49" t="s">
         <v>76</v>
@@ -9102,7 +9103,7 @@
     </row>
     <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B50" t="s">
         <v>70</v>
@@ -9141,7 +9142,7 @@
         <v>92</v>
       </c>
       <c r="N50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O50" t="s">
         <v>387</v>
@@ -9231,7 +9232,7 @@
         <v>60.373251066259371</v>
       </c>
       <c r="AR50" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AS50" t="s">
         <v>115</v>
@@ -9242,7 +9243,7 @@
     </row>
     <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B51" t="s">
         <v>70</v>
@@ -9374,7 +9375,7 @@
         <v>65</v>
       </c>
       <c r="AS51" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AT51" t="s">
         <v>76</v>
@@ -9382,7 +9383,7 @@
     </row>
     <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B52" t="s">
         <v>70</v>
@@ -9421,7 +9422,7 @@
         <v>69</v>
       </c>
       <c r="N52" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="O52" t="s">
         <v>387</v>
@@ -9511,10 +9512,10 @@
         <v>77.694406134559856</v>
       </c>
       <c r="AR52" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="AS52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AT52" t="s">
         <v>76</v>
@@ -9662,7 +9663,7 @@
     </row>
     <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B54" t="s">
         <v>70</v>
@@ -9683,7 +9684,7 @@
         <v>80</v>
       </c>
       <c r="H54" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I54" t="s">
         <v>65</v>
@@ -9701,10 +9702,10 @@
         <v>92</v>
       </c>
       <c r="N54" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="O54" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="P54" t="s">
         <v>65</v>
@@ -9791,10 +9792,10 @@
         <v>78.767922997520941</v>
       </c>
       <c r="AR54" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AS54" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AT54" t="s">
         <v>76</v>
@@ -9802,7 +9803,7 @@
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B55" t="s">
         <v>70</v>
@@ -9826,7 +9827,7 @@
         <v>65</v>
       </c>
       <c r="I55" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J55" t="s">
         <v>138</v>
@@ -9841,7 +9842,7 @@
         <v>114</v>
       </c>
       <c r="N55" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="O55" t="s">
         <v>65</v>
@@ -9934,10 +9935,10 @@
         <v>65</v>
       </c>
       <c r="AS55" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="AT55" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.25">
@@ -10222,7 +10223,7 @@
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B58" t="s">
         <v>70</v>
@@ -10261,7 +10262,7 @@
         <v>193</v>
       </c>
       <c r="N58" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="O58" t="s">
         <v>65</v>
@@ -10351,10 +10352,10 @@
         <v>66.16033056179792</v>
       </c>
       <c r="AR58" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="AS58" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AT58" t="s">
         <v>76</v>
@@ -10502,7 +10503,7 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
@@ -10541,7 +10542,7 @@
         <v>92</v>
       </c>
       <c r="N60" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O60" t="s">
         <v>65</v>
@@ -10642,7 +10643,7 @@
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B61" t="s">
         <v>70</v>
@@ -10681,7 +10682,7 @@
         <v>69</v>
       </c>
       <c r="N61" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="O61" t="s">
         <v>298</v>
@@ -10770,11 +10771,11 @@
       <c r="AQ61">
         <v>61.989585934321688</v>
       </c>
-      <c r="AR61" t="s">
-        <v>455</v>
+      <c r="AR61" s="1" t="s">
+        <v>625</v>
       </c>
       <c r="AS61" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AT61" t="s">
         <v>76</v>
@@ -10922,7 +10923,7 @@
     </row>
     <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B63" t="s">
         <v>70</v>
@@ -10961,7 +10962,7 @@
         <v>114</v>
       </c>
       <c r="N63" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="O63" t="s">
         <v>65</v>
@@ -11051,10 +11052,10 @@
         <v>96.04634212554906</v>
       </c>
       <c r="AR63" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="AS63" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="AT63" t="s">
         <v>76</v>
@@ -11482,7 +11483,7 @@
     </row>
     <row r="67" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -11521,7 +11522,7 @@
         <v>92</v>
       </c>
       <c r="N67" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O67" t="s">
         <v>65</v>
@@ -11902,7 +11903,7 @@
     </row>
     <row r="70" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B70" t="s">
         <v>70</v>
@@ -11926,7 +11927,7 @@
         <v>65</v>
       </c>
       <c r="I70" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J70" t="s">
         <v>136</v>
@@ -12030,8 +12031,8 @@
       <c r="AQ70">
         <v>59.033144078614221</v>
       </c>
-      <c r="AR70" t="s">
-        <v>410</v>
+      <c r="AR70" s="1" t="s">
+        <v>624</v>
       </c>
       <c r="AS70" t="s">
         <v>75</v>
@@ -12182,7 +12183,7 @@
     </row>
     <row r="72" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
@@ -12221,7 +12222,7 @@
         <v>107</v>
       </c>
       <c r="N72" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="O72" t="s">
         <v>65</v>
@@ -12462,7 +12463,7 @@
     </row>
     <row r="74" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B74" t="s">
         <v>70</v>
@@ -12594,7 +12595,7 @@
         <v>65</v>
       </c>
       <c r="AS74" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="AT74" t="s">
         <v>76</v>
@@ -12882,7 +12883,7 @@
     </row>
     <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B77" t="s">
         <v>70</v>
@@ -12921,7 +12922,7 @@
         <v>107</v>
       </c>
       <c r="N77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O77" t="s">
         <v>65</v>
@@ -13302,7 +13303,7 @@
     </row>
     <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B80" t="s">
         <v>70</v>
@@ -13434,7 +13435,7 @@
         <v>65</v>
       </c>
       <c r="AS80" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AT80" t="s">
         <v>76</v>
@@ -13442,7 +13443,7 @@
     </row>
     <row r="81" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B81" t="s">
         <v>70</v>
@@ -13481,7 +13482,7 @@
         <v>107</v>
       </c>
       <c r="N81" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="O81" t="s">
         <v>65</v>
@@ -13574,7 +13575,7 @@
         <v>65</v>
       </c>
       <c r="AS81" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="AT81" t="s">
         <v>76</v>
@@ -14142,7 +14143,7 @@
     </row>
     <row r="86" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B86" t="s">
         <v>70</v>
@@ -14181,7 +14182,7 @@
         <v>92</v>
       </c>
       <c r="N86" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="O86" t="s">
         <v>65</v>
@@ -14282,7 +14283,7 @@
     </row>
     <row r="87" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B87" t="s">
         <v>70</v>
@@ -14414,7 +14415,7 @@
         <v>65</v>
       </c>
       <c r="AS87" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="AT87" t="s">
         <v>76</v>
@@ -14422,7 +14423,7 @@
     </row>
     <row r="88" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B88" t="s">
         <v>70</v>
@@ -14443,7 +14444,7 @@
         <v>180</v>
       </c>
       <c r="H88" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I88" t="s">
         <v>65</v>
@@ -14461,7 +14462,7 @@
         <v>107</v>
       </c>
       <c r="N88" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O88" t="s">
         <v>298</v>
@@ -14551,10 +14552,10 @@
         <v>71.56359557518887</v>
       </c>
       <c r="AR88" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AS88" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AT88" t="s">
         <v>76</v>
@@ -14562,7 +14563,7 @@
     </row>
     <row r="89" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B89" t="s">
         <v>70</v>
@@ -14601,7 +14602,7 @@
         <v>114</v>
       </c>
       <c r="N89" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="O89" t="s">
         <v>65</v>
@@ -14692,7 +14693,7 @@
         <v>65</v>
       </c>
       <c r="AS89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AT89" t="s">
         <v>76</v>
@@ -14837,7 +14838,7 @@
     </row>
     <row r="91" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B91" t="s">
         <v>70</v>
@@ -14882,7 +14883,7 @@
         <v>65</v>
       </c>
       <c r="P91" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="Q91" t="s">
         <v>70</v>
@@ -14969,10 +14970,10 @@
         <v>65</v>
       </c>
       <c r="AS91" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AT91" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="92" spans="1:46" x14ac:dyDescent="0.25">
@@ -15117,7 +15118,7 @@
     </row>
     <row r="93" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B93" t="s">
         <v>70</v>
@@ -15138,10 +15139,10 @@
         <v>64</v>
       </c>
       <c r="H93" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I93" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J93" t="s">
         <v>272</v>
@@ -15156,7 +15157,7 @@
         <v>107</v>
       </c>
       <c r="N93" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="O93" t="s">
         <v>65</v>
@@ -15246,10 +15247,10 @@
         <v>68.047673831587403</v>
       </c>
       <c r="AR93" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="AS93" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AT93" t="s">
         <v>76</v>
@@ -15257,7 +15258,7 @@
     </row>
     <row r="94" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B94" t="s">
         <v>70</v>
@@ -15281,7 +15282,7 @@
         <v>65</v>
       </c>
       <c r="I94" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J94" t="s">
         <v>141</v>
@@ -15296,7 +15297,7 @@
         <v>114</v>
       </c>
       <c r="N94" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O94" t="s">
         <v>65</v>
@@ -15386,10 +15387,10 @@
         <v>82.410667961035145</v>
       </c>
       <c r="AR94" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AS94" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="AT94" t="s">
         <v>76</v>
@@ -15397,7 +15398,7 @@
     </row>
     <row r="95" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B95" t="s">
         <v>70</v>
@@ -15418,10 +15419,10 @@
         <v>64</v>
       </c>
       <c r="H95" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I95" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J95" t="s">
         <v>124</v>
@@ -15436,7 +15437,7 @@
         <v>92</v>
       </c>
       <c r="N95" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="O95" t="s">
         <v>65</v>
@@ -15526,10 +15527,10 @@
         <v>76.454145985162981</v>
       </c>
       <c r="AR95" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AS95" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AT95" t="s">
         <v>76</v>
@@ -15537,7 +15538,7 @@
     </row>
     <row r="96" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B96" t="s">
         <v>70</v>
@@ -15561,7 +15562,7 @@
         <v>65</v>
       </c>
       <c r="I96" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J96" t="s">
         <v>365</v>
@@ -15576,7 +15577,7 @@
         <v>92</v>
       </c>
       <c r="N96" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="O96" t="s">
         <v>65</v>
@@ -15669,7 +15670,7 @@
         <v>65</v>
       </c>
       <c r="AS96" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AT96" t="s">
         <v>76</v>
@@ -15677,7 +15678,7 @@
     </row>
     <row r="97" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B97" t="s">
         <v>70</v>
@@ -15716,7 +15717,7 @@
         <v>92</v>
       </c>
       <c r="N97" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="O97" t="s">
         <v>298</v>
@@ -15806,10 +15807,10 @@
         <v>88.929493477207373</v>
       </c>
       <c r="AR97" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="AS97" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AT97" t="s">
         <v>76</v>
@@ -15957,7 +15958,7 @@
     </row>
     <row r="99" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B99" t="s">
         <v>70</v>
@@ -15996,7 +15997,7 @@
         <v>107</v>
       </c>
       <c r="N99" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O99" t="s">
         <v>298</v>
@@ -16029,7 +16030,7 @@
         <v>65</v>
       </c>
       <c r="Y99" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Z99">
         <v>2003</v>
@@ -16086,7 +16087,7 @@
         <v>60.373251066259371</v>
       </c>
       <c r="AR99" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AS99" t="s">
         <v>308</v>

</xml_diff>